<commit_message>
Ajout de documents consultables
</commit_message>
<xml_diff>
--- a/Document E4 MEZAOUI Alex Sofiane.xlsx
+++ b/Document E4 MEZAOUI Alex Sofiane.xlsx
@@ -5,25 +5,25 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sofiane\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sofiane\Documents\GitHub\AlexMezaoui.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E5F70BA-39BB-4D0A-8DBD-E91D5ADF2DDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36F759EB-9AB1-4607-9880-6979DD5CDF84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3240" yWindow="3240" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tableau de synthèse Épreuve E4" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Tableau de synthèse Épreuve E4'!$A$1:$H$36</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Tableau de synthèse Épreuve E4'!$A$1:$H$35</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
   <si>
     <t>Gérer le patrimoine informatique</t>
   </si>
@@ -131,25 +131,13 @@
     <t>Projet Personnel</t>
   </si>
   <si>
-    <t>Veille Technologique : Linus ASAHI</t>
-  </si>
-  <si>
-    <t>Déploiement d'un site avec apache2</t>
-  </si>
-  <si>
-    <t>TP Fail2Ban et Patator</t>
-  </si>
-  <si>
     <t>Portfolio</t>
   </si>
   <si>
-    <t>Connexion API</t>
-  </si>
-  <si>
-    <t>Réalisation d'une applaction web, en lien avec l'API de chat GPT</t>
-  </si>
-  <si>
-    <t>SS</t>
+    <t>TP GLPI Gestion d'incidents</t>
+  </si>
+  <si>
+    <t>Veille Technologique : Linux ASAHI</t>
   </si>
 </sst>
 </file>
@@ -585,9 +573,51 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="11" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -596,48 +626,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="11" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1012,10 +1000,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AQ82"/>
+  <dimension ref="A1:AQ81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1028,56 +1016,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22" t="s">
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="22"/>
+      <c r="H1" s="28"/>
     </row>
     <row r="2" spans="1:43" ht="41.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
     </row>
     <row r="3" spans="1:43" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="23" t="s">
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="24"/>
-      <c r="H3" s="25"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="39"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:43" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="25"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="39"/>
       <c r="F4" s="14" t="s">
         <v>8</v>
       </c>
@@ -1092,7 +1080,7 @@
       <c r="A5" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="35" t="s">
         <v>20</v>
       </c>
       <c r="C5" s="6" t="s">
@@ -1116,7 +1104,7 @@
     </row>
     <row r="6" spans="1:43" s="2" customFormat="1" ht="324.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="27"/>
-      <c r="B6" s="35"/>
+      <c r="B6" s="36"/>
       <c r="C6" s="8" t="s">
         <v>9</v>
       </c>
@@ -1172,16 +1160,16 @@
       <c r="AQ6"/>
     </row>
     <row r="7" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A7" s="28" t="s">
+      <c r="A7" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="29"/>
-      <c r="C7" s="29"/>
-      <c r="D7" s="29"/>
-      <c r="E7" s="29"/>
-      <c r="F7" s="29"/>
-      <c r="G7" s="29"/>
-      <c r="H7" s="30"/>
+      <c r="B7" s="30"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="31"/>
       <c r="I7"/>
       <c r="J7"/>
       <c r="K7"/>
@@ -1223,7 +1211,7 @@
         <v>26</v>
       </c>
       <c r="B8" s="10"/>
-      <c r="C8" s="36" t="s">
+      <c r="C8" s="22" t="s">
         <v>27</v>
       </c>
       <c r="D8" s="17"/>
@@ -1275,10 +1263,10 @@
       <c r="C9" s="17"/>
       <c r="D9" s="17"/>
       <c r="E9" s="18"/>
-      <c r="F9" s="36" t="s">
+      <c r="F9" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="G9" s="36" t="s">
+      <c r="G9" s="22" t="s">
         <v>27</v>
       </c>
       <c r="H9" s="19"/>
@@ -1320,7 +1308,7 @@
     </row>
     <row r="10" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B10" s="10"/>
       <c r="C10" s="18"/>
@@ -1328,7 +1316,7 @@
       <c r="E10" s="18"/>
       <c r="F10" s="18"/>
       <c r="G10" s="17"/>
-      <c r="H10" s="37" t="s">
+      <c r="H10" s="23" t="s">
         <v>27</v>
       </c>
       <c r="I10"/>
@@ -1371,12 +1359,12 @@
       <c r="A11" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="10"/>
+      <c r="B11" s="17"/>
       <c r="C11" s="17"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="36" t="s">
+      <c r="D11" s="22" t="s">
         <v>27</v>
       </c>
+      <c r="E11" s="18"/>
       <c r="F11" s="18"/>
       <c r="G11" s="17"/>
       <c r="H11" s="19"/>
@@ -1418,17 +1406,19 @@
     </row>
     <row r="12" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="10"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="E12" s="18"/>
       <c r="F12" s="18"/>
       <c r="G12" s="17"/>
-      <c r="H12" s="19"/>
+      <c r="H12" s="25" t="s">
+        <v>27</v>
+      </c>
       <c r="I12"/>
       <c r="J12"/>
       <c r="K12"/>
@@ -1466,20 +1456,14 @@
       <c r="AQ12"/>
     </row>
     <row r="13" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="11" t="s">
-        <v>32</v>
-      </c>
+      <c r="A13" s="11"/>
       <c r="B13" s="10"/>
-      <c r="C13" s="18"/>
+      <c r="C13" s="17"/>
       <c r="D13" s="18"/>
-      <c r="E13" s="38" t="s">
-        <v>27</v>
-      </c>
-      <c r="F13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="17"/>
       <c r="G13" s="17"/>
-      <c r="H13" s="39" t="s">
-        <v>27</v>
-      </c>
+      <c r="H13" s="19"/>
       <c r="I13"/>
       <c r="J13"/>
       <c r="K13"/>
@@ -1519,11 +1503,11 @@
     <row r="14" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="11"/>
       <c r="B14" s="10"/>
-      <c r="C14" s="17"/>
+      <c r="C14" s="18"/>
       <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
       <c r="H14" s="19"/>
       <c r="I14"/>
       <c r="J14"/>
@@ -1566,7 +1550,7 @@
       <c r="B15" s="10"/>
       <c r="C15" s="18"/>
       <c r="D15" s="18"/>
-      <c r="E15" s="17"/>
+      <c r="E15" s="18"/>
       <c r="F15" s="18"/>
       <c r="G15" s="18"/>
       <c r="H15" s="19"/>
@@ -1651,15 +1635,17 @@
       <c r="AP16"/>
       <c r="AQ16"/>
     </row>
-    <row r="17" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="11"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="19"/>
+    <row r="17" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A17" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="33"/>
+      <c r="C17" s="33"/>
+      <c r="D17" s="33"/>
+      <c r="E17" s="33"/>
+      <c r="F17" s="33"/>
+      <c r="G17" s="33"/>
+      <c r="H17" s="34"/>
       <c r="I17"/>
       <c r="J17"/>
       <c r="K17"/>
@@ -1696,17 +1682,15 @@
       <c r="AP17"/>
       <c r="AQ17"/>
     </row>
-    <row r="18" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A18" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="B18" s="32"/>
-      <c r="C18" s="32"/>
-      <c r="D18" s="32"/>
-      <c r="E18" s="32"/>
-      <c r="F18" s="32"/>
-      <c r="G18" s="32"/>
-      <c r="H18" s="33"/>
+    <row r="18" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="11"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="19"/>
       <c r="I18"/>
       <c r="J18"/>
       <c r="K18"/>
@@ -1744,17 +1728,13 @@
       <c r="AQ18"/>
     </row>
     <row r="19" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="B19" s="17"/>
+      <c r="A19" s="11"/>
+      <c r="B19" s="10"/>
       <c r="C19" s="17"/>
-      <c r="D19" s="18"/>
+      <c r="D19" s="17"/>
       <c r="E19" s="18"/>
-      <c r="F19" s="36" t="s">
-        <v>27</v>
-      </c>
-      <c r="G19" s="17"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="22"/>
       <c r="H19" s="19"/>
       <c r="I19"/>
       <c r="J19"/>
@@ -1793,19 +1773,13 @@
       <c r="AQ19"/>
     </row>
     <row r="20" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="11" t="s">
-        <v>34</v>
-      </c>
+      <c r="A20" s="11"/>
       <c r="B20" s="10"/>
       <c r="C20" s="17"/>
       <c r="D20" s="17"/>
       <c r="E20" s="18"/>
-      <c r="F20" s="36" t="s">
-        <v>35</v>
-      </c>
-      <c r="G20" s="36" t="s">
-        <v>27</v>
-      </c>
+      <c r="F20" s="18"/>
+      <c r="G20" s="17"/>
       <c r="H20" s="19"/>
       <c r="I20"/>
       <c r="J20"/>
@@ -1845,12 +1819,12 @@
     </row>
     <row r="21" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="11"/>
-      <c r="B21" s="10"/>
+      <c r="B21" s="17"/>
       <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
+      <c r="D21" s="18"/>
       <c r="E21" s="18"/>
       <c r="F21" s="18"/>
-      <c r="G21" s="17"/>
+      <c r="G21" s="18"/>
       <c r="H21" s="19"/>
       <c r="I21"/>
       <c r="J21"/>
@@ -1890,11 +1864,11 @@
     </row>
     <row r="22" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="11"/>
-      <c r="B22" s="17"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="18"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="17"/>
       <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
+      <c r="F22" s="17"/>
       <c r="G22" s="18"/>
       <c r="H22" s="19"/>
       <c r="I22"/>
@@ -1982,9 +1956,9 @@
       <c r="A24" s="11"/>
       <c r="B24" s="10"/>
       <c r="C24" s="18"/>
-      <c r="D24" s="17"/>
+      <c r="D24" s="18"/>
       <c r="E24" s="18"/>
-      <c r="F24" s="17"/>
+      <c r="F24" s="18"/>
       <c r="G24" s="18"/>
       <c r="H24" s="19"/>
       <c r="I24"/>
@@ -2068,15 +2042,17 @@
       <c r="AP25"/>
       <c r="AQ25"/>
     </row>
-    <row r="26" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="11"/>
-      <c r="B26" s="10"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
-      <c r="H26" s="19"/>
+    <row r="26" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A26" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="B26" s="33"/>
+      <c r="C26" s="33"/>
+      <c r="D26" s="33"/>
+      <c r="E26" s="33"/>
+      <c r="F26" s="33"/>
+      <c r="G26" s="33"/>
+      <c r="H26" s="34"/>
       <c r="I26"/>
       <c r="J26"/>
       <c r="K26"/>
@@ -2113,17 +2089,15 @@
       <c r="AP26"/>
       <c r="AQ26"/>
     </row>
-    <row r="27" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A27" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="B27" s="32"/>
-      <c r="C27" s="32"/>
-      <c r="D27" s="32"/>
-      <c r="E27" s="32"/>
-      <c r="F27" s="32"/>
-      <c r="G27" s="32"/>
-      <c r="H27" s="33"/>
+    <row r="27" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="11"/>
+      <c r="B27" s="10"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="19"/>
       <c r="I27"/>
       <c r="J27"/>
       <c r="K27"/>
@@ -2430,15 +2404,15 @@
       <c r="AP33"/>
       <c r="AQ33"/>
     </row>
-    <row r="34" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="11"/>
-      <c r="B34" s="10"/>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
-      <c r="G34" s="18"/>
-      <c r="H34" s="19"/>
+    <row r="34" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="12"/>
+      <c r="B34" s="13"/>
+      <c r="C34" s="20"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="20"/>
+      <c r="F34" s="20"/>
+      <c r="G34" s="20"/>
+      <c r="H34" s="21"/>
       <c r="I34"/>
       <c r="J34"/>
       <c r="K34"/>
@@ -2475,15 +2449,15 @@
       <c r="AP34"/>
       <c r="AQ34"/>
     </row>
-    <row r="35" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="12"/>
-      <c r="B35" s="13"/>
-      <c r="C35" s="20"/>
-      <c r="D35" s="20"/>
-      <c r="E35" s="20"/>
-      <c r="F35" s="20"/>
-      <c r="G35" s="20"/>
-      <c r="H35" s="21"/>
+    <row r="35" spans="1:43" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A35" s="5"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4"/>
+      <c r="H35" s="4"/>
       <c r="I35"/>
       <c r="J35"/>
       <c r="K35"/>
@@ -2520,51 +2494,7 @@
       <c r="AP35"/>
       <c r="AQ35"/>
     </row>
-    <row r="36" spans="1:43" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A36" s="5"/>
-      <c r="B36" s="3"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="4"/>
-      <c r="G36" s="4"/>
-      <c r="H36" s="4"/>
-      <c r="I36"/>
-      <c r="J36"/>
-      <c r="K36"/>
-      <c r="L36"/>
-      <c r="M36"/>
-      <c r="N36"/>
-      <c r="O36"/>
-      <c r="P36"/>
-      <c r="Q36"/>
-      <c r="R36"/>
-      <c r="S36"/>
-      <c r="T36"/>
-      <c r="U36"/>
-      <c r="V36"/>
-      <c r="W36"/>
-      <c r="X36"/>
-      <c r="Y36"/>
-      <c r="Z36"/>
-      <c r="AA36"/>
-      <c r="AB36"/>
-      <c r="AC36"/>
-      <c r="AD36"/>
-      <c r="AE36"/>
-      <c r="AF36"/>
-      <c r="AG36"/>
-      <c r="AH36"/>
-      <c r="AI36"/>
-      <c r="AJ36"/>
-      <c r="AK36"/>
-      <c r="AL36"/>
-      <c r="AM36"/>
-      <c r="AN36"/>
-      <c r="AO36"/>
-      <c r="AP36"/>
-      <c r="AQ36"/>
-    </row>
+    <row r="36" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="37" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="38" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="39" spans="1:43" customFormat="1" x14ac:dyDescent="0.2"/>
@@ -2610,20 +2540,19 @@
     <row r="79" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="80" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="81" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="82" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A7:H7"/>
-    <mergeCell ref="A18:H18"/>
-    <mergeCell ref="A27:H27"/>
-    <mergeCell ref="B5:B6"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A3:E3"/>
     <mergeCell ref="A4:E4"/>
     <mergeCell ref="F3:H3"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A7:H7"/>
+    <mergeCell ref="A17:H17"/>
+    <mergeCell ref="A26:H26"/>
+    <mergeCell ref="B5:B6"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>

<commit_message>
Update Document E4 MEZAOUI Alex Sofiane.xlsx
</commit_message>
<xml_diff>
--- a/Document E4 MEZAOUI Alex Sofiane.xlsx
+++ b/Document E4 MEZAOUI Alex Sofiane.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sofiane\Documents\GitHub\AlexMezaoui.github.io\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2CA138A-0A4F-4B0B-AE1D-3A4FCB3F01BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3240" yWindow="3240" windowWidth="21600" windowHeight="11385"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tableau de synthèse Épreuve E4" sheetId="1" r:id="rId1"/>
@@ -17,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="43">
   <si>
     <t>Gérer le patrimoine informatique</t>
   </si>
@@ -163,15 +169,18 @@
   <si>
     <t>04/09/2023 au 24/04/2024</t>
   </si>
+  <si>
+    <t>Entièrete de ma scolarité</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00\ [$€-1]_-;\-* #,##0.00\ [$€-1]_-;_-* &quot;-&quot;??\ [$€-1]_-"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -573,15 +582,24 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -606,18 +624,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Euro" xfId="1"/>
+    <cellStyle name="Euro" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -653,7 +662,7 @@
         <xdr:cNvPr id="2" name="Organigramme : Jonction de sommaire 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B476B94D-B515-934C-9F03-5349E8AEF44C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B476B94D-B515-934C-9F03-5349E8AEF44C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -699,9 +708,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -739,7 +748,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -773,6 +782,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -807,9 +817,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -982,17 +993,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:AQ65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="70.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="11.7109375" style="27" customWidth="1"/>
@@ -1001,57 +1012,57 @@
     <col min="44" max="16384" width="10.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" ht="39.950000000000003" customHeight="1">
-      <c r="A1" s="31" t="s">
+    <row r="1" spans="1:43" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31" t="s">
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="H1" s="31"/>
-    </row>
-    <row r="2" spans="1:43" ht="41.1" customHeight="1">
-      <c r="A2" s="31" t="s">
+      <c r="H1" s="29"/>
+    </row>
+    <row r="2" spans="1:43" ht="41.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-    </row>
-    <row r="3" spans="1:43" ht="39.950000000000003" customHeight="1">
-      <c r="A3" s="40" t="s">
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+    </row>
+    <row r="3" spans="1:43" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="41"/>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="40" t="s">
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="41"/>
-      <c r="H3" s="42"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="32"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
-    <row r="4" spans="1:43" ht="39.950000000000003" customHeight="1" thickBot="1">
-      <c r="A4" s="40" t="s">
+    <row r="4" spans="1:43" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="B4" s="41"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="41"/>
-      <c r="E4" s="42"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="32"/>
       <c r="F4" s="10" t="s">
         <v>8</v>
       </c>
@@ -1062,11 +1073,11 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:43" ht="90" customHeight="1">
-      <c r="A5" s="29" t="s">
+    <row r="5" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="38" t="s">
+      <c r="B5" s="41" t="s">
         <v>20</v>
       </c>
       <c r="C5" s="5" t="s">
@@ -1088,9 +1099,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:43" s="2" customFormat="1" ht="324.95" customHeight="1" thickBot="1">
-      <c r="A6" s="30"/>
-      <c r="B6" s="39"/>
+    <row r="6" spans="1:43" s="2" customFormat="1" ht="324.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="34"/>
+      <c r="B6" s="42"/>
       <c r="C6" s="7" t="s">
         <v>9</v>
       </c>
@@ -1145,17 +1156,17 @@
       <c r="AP6"/>
       <c r="AQ6"/>
     </row>
-    <row r="7" spans="1:43" s="2" customFormat="1" ht="18">
-      <c r="A7" s="32" t="s">
+    <row r="7" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A7" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="33"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="33"/>
-      <c r="G7" s="33"/>
-      <c r="H7" s="34"/>
+      <c r="B7" s="36"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="36"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="36"/>
+      <c r="H7" s="37"/>
       <c r="I7"/>
       <c r="J7"/>
       <c r="K7"/>
@@ -1192,7 +1203,7 @@
       <c r="AP7"/>
       <c r="AQ7"/>
     </row>
-    <row r="8" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1">
+    <row r="8" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
         <v>24</v>
       </c>
@@ -1243,7 +1254,7 @@
       <c r="AP8"/>
       <c r="AQ8"/>
     </row>
-    <row r="9" spans="1:43" s="2" customFormat="1" ht="48" customHeight="1">
+    <row r="9" spans="1:43" s="2" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
         <v>26</v>
       </c>
@@ -1296,7 +1307,7 @@
       <c r="AP9"/>
       <c r="AQ9"/>
     </row>
-    <row r="10" spans="1:43" s="2" customFormat="1" ht="47.25" customHeight="1">
+    <row r="10" spans="1:43" s="2" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
         <v>29</v>
       </c>
@@ -1347,7 +1358,7 @@
       <c r="AP10"/>
       <c r="AQ10"/>
     </row>
-    <row r="11" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1">
+    <row r="11" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
         <v>28</v>
       </c>
@@ -1398,12 +1409,12 @@
       <c r="AP11"/>
       <c r="AQ11"/>
     </row>
-    <row r="12" spans="1:43" s="2" customFormat="1" ht="44.25" customHeight="1">
+    <row r="12" spans="1:43" s="2" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
         <v>27</v>
       </c>
       <c r="B12" s="25" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="C12" s="18"/>
       <c r="D12" s="18"/>
@@ -1449,7 +1460,7 @@
       <c r="AP12"/>
       <c r="AQ12"/>
     </row>
-    <row r="13" spans="1:43" s="2" customFormat="1" ht="45.75" customHeight="1">
+    <row r="13" spans="1:43" s="2" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
         <v>30</v>
       </c>
@@ -1502,7 +1513,7 @@
       <c r="AP13"/>
       <c r="AQ13"/>
     </row>
-    <row r="14" spans="1:43" s="2" customFormat="1" ht="48" customHeight="1">
+    <row r="14" spans="1:43" s="2" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="9" t="s">
         <v>32</v>
       </c>
@@ -1555,17 +1566,17 @@
       <c r="AP14"/>
       <c r="AQ14"/>
     </row>
-    <row r="15" spans="1:43" s="2" customFormat="1" ht="18">
-      <c r="A15" s="35" t="s">
+    <row r="15" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A15" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="36"/>
-      <c r="C15" s="36"/>
-      <c r="D15" s="36"/>
-      <c r="E15" s="36"/>
-      <c r="F15" s="36"/>
-      <c r="G15" s="36"/>
-      <c r="H15" s="37"/>
+      <c r="B15" s="39"/>
+      <c r="C15" s="39"/>
+      <c r="D15" s="39"/>
+      <c r="E15" s="39"/>
+      <c r="F15" s="39"/>
+      <c r="G15" s="39"/>
+      <c r="H15" s="40"/>
       <c r="I15"/>
       <c r="J15"/>
       <c r="K15"/>
@@ -1602,7 +1613,7 @@
       <c r="AP15"/>
       <c r="AQ15"/>
     </row>
-    <row r="16" spans="1:43" s="2" customFormat="1" ht="45" customHeight="1">
+    <row r="16" spans="1:43" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
         <v>31</v>
       </c>
@@ -1655,17 +1666,17 @@
       <c r="AP16"/>
       <c r="AQ16"/>
     </row>
-    <row r="17" spans="1:43" s="2" customFormat="1" ht="18">
-      <c r="A17" s="35" t="s">
+    <row r="17" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A17" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="36"/>
-      <c r="C17" s="36"/>
-      <c r="D17" s="36"/>
-      <c r="E17" s="36"/>
-      <c r="F17" s="36"/>
-      <c r="G17" s="36"/>
-      <c r="H17" s="37"/>
+      <c r="B17" s="39"/>
+      <c r="C17" s="39"/>
+      <c r="D17" s="39"/>
+      <c r="E17" s="39"/>
+      <c r="F17" s="39"/>
+      <c r="G17" s="39"/>
+      <c r="H17" s="40"/>
       <c r="I17"/>
       <c r="J17"/>
       <c r="K17"/>
@@ -1702,7 +1713,7 @@
       <c r="AP17"/>
       <c r="AQ17"/>
     </row>
-    <row r="18" spans="1:43" s="2" customFormat="1" ht="44.25" customHeight="1">
+    <row r="18" spans="1:43" s="2" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
         <v>36</v>
       </c>
@@ -1755,7 +1766,7 @@
       <c r="AP18"/>
       <c r="AQ18"/>
     </row>
-    <row r="19" spans="1:43" s="2" customFormat="1">
+    <row r="19" spans="1:43" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4"/>
       <c r="B19" s="27"/>
       <c r="C19" s="3"/>
@@ -1800,157 +1811,157 @@
       <c r="AP19"/>
       <c r="AQ19"/>
     </row>
-    <row r="20" spans="1:43" customFormat="1">
+    <row r="20" spans="1:43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B20" s="28"/>
     </row>
-    <row r="21" spans="1:43" customFormat="1">
+    <row r="21" spans="1:43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="28"/>
     </row>
-    <row r="22" spans="1:43" customFormat="1">
+    <row r="22" spans="1:43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B22" s="28"/>
     </row>
-    <row r="23" spans="1:43" customFormat="1">
+    <row r="23" spans="1:43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="28"/>
     </row>
-    <row r="24" spans="1:43" customFormat="1">
+    <row r="24" spans="1:43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B24" s="28"/>
     </row>
-    <row r="25" spans="1:43" customFormat="1">
+    <row r="25" spans="1:43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B25" s="28"/>
     </row>
-    <row r="26" spans="1:43" customFormat="1">
+    <row r="26" spans="1:43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B26" s="28"/>
     </row>
-    <row r="27" spans="1:43" customFormat="1">
+    <row r="27" spans="1:43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B27" s="28"/>
     </row>
-    <row r="28" spans="1:43" customFormat="1">
+    <row r="28" spans="1:43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B28" s="28"/>
     </row>
-    <row r="29" spans="1:43" customFormat="1">
+    <row r="29" spans="1:43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B29" s="28"/>
     </row>
-    <row r="30" spans="1:43" customFormat="1">
+    <row r="30" spans="1:43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B30" s="28"/>
     </row>
-    <row r="31" spans="1:43" customFormat="1">
+    <row r="31" spans="1:43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B31" s="28"/>
     </row>
-    <row r="32" spans="1:43" customFormat="1">
+    <row r="32" spans="1:43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B32" s="28"/>
     </row>
-    <row r="33" spans="2:2" customFormat="1">
+    <row r="33" spans="2:2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B33" s="28"/>
     </row>
-    <row r="34" spans="2:2" customFormat="1">
+    <row r="34" spans="2:2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B34" s="28"/>
     </row>
-    <row r="35" spans="2:2" customFormat="1">
+    <row r="35" spans="2:2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B35" s="28"/>
     </row>
-    <row r="36" spans="2:2" customFormat="1">
+    <row r="36" spans="2:2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B36" s="28"/>
     </row>
-    <row r="37" spans="2:2" customFormat="1">
+    <row r="37" spans="2:2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B37" s="28"/>
     </row>
-    <row r="38" spans="2:2" customFormat="1">
+    <row r="38" spans="2:2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B38" s="28"/>
     </row>
-    <row r="39" spans="2:2" customFormat="1">
+    <row r="39" spans="2:2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B39" s="28"/>
     </row>
-    <row r="40" spans="2:2" customFormat="1">
+    <row r="40" spans="2:2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B40" s="28"/>
     </row>
-    <row r="41" spans="2:2" customFormat="1">
+    <row r="41" spans="2:2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B41" s="28"/>
     </row>
-    <row r="42" spans="2:2" customFormat="1">
+    <row r="42" spans="2:2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B42" s="28"/>
     </row>
-    <row r="43" spans="2:2" customFormat="1">
+    <row r="43" spans="2:2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B43" s="28"/>
     </row>
-    <row r="44" spans="2:2" customFormat="1">
+    <row r="44" spans="2:2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B44" s="28"/>
     </row>
-    <row r="45" spans="2:2" customFormat="1">
+    <row r="45" spans="2:2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B45" s="28"/>
     </row>
-    <row r="46" spans="2:2" customFormat="1">
+    <row r="46" spans="2:2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B46" s="28"/>
     </row>
-    <row r="47" spans="2:2" customFormat="1">
+    <row r="47" spans="2:2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B47" s="28"/>
     </row>
-    <row r="48" spans="2:2" customFormat="1">
+    <row r="48" spans="2:2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B48" s="28"/>
     </row>
-    <row r="49" spans="2:2" customFormat="1">
+    <row r="49" spans="2:2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B49" s="28"/>
     </row>
-    <row r="50" spans="2:2" customFormat="1">
+    <row r="50" spans="2:2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B50" s="28"/>
     </row>
-    <row r="51" spans="2:2" customFormat="1">
+    <row r="51" spans="2:2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B51" s="28"/>
     </row>
-    <row r="52" spans="2:2" customFormat="1">
+    <row r="52" spans="2:2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B52" s="28"/>
     </row>
-    <row r="53" spans="2:2" customFormat="1">
+    <row r="53" spans="2:2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B53" s="28"/>
     </row>
-    <row r="54" spans="2:2" customFormat="1">
+    <row r="54" spans="2:2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B54" s="28"/>
     </row>
-    <row r="55" spans="2:2" customFormat="1">
+    <row r="55" spans="2:2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B55" s="28"/>
     </row>
-    <row r="56" spans="2:2" customFormat="1">
+    <row r="56" spans="2:2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B56" s="28"/>
     </row>
-    <row r="57" spans="2:2" customFormat="1">
+    <row r="57" spans="2:2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B57" s="28"/>
     </row>
-    <row r="58" spans="2:2" customFormat="1">
+    <row r="58" spans="2:2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B58" s="28"/>
     </row>
-    <row r="59" spans="2:2" customFormat="1">
+    <row r="59" spans="2:2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B59" s="28"/>
     </row>
-    <row r="60" spans="2:2" customFormat="1">
+    <row r="60" spans="2:2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B60" s="28"/>
     </row>
-    <row r="61" spans="2:2" customFormat="1">
+    <row r="61" spans="2:2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B61" s="28"/>
     </row>
-    <row r="62" spans="2:2" customFormat="1">
+    <row r="62" spans="2:2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B62" s="28"/>
     </row>
-    <row r="63" spans="2:2" customFormat="1">
+    <row r="63" spans="2:2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B63" s="28"/>
     </row>
-    <row r="64" spans="2:2" customFormat="1">
+    <row r="64" spans="2:2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B64" s="28"/>
     </row>
-    <row r="65" spans="2:2" customFormat="1">
+    <row r="65" spans="2:2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B65" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="F3:H3"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A7:H7"/>
     <mergeCell ref="A15:H15"/>
     <mergeCell ref="A17:H17"/>
     <mergeCell ref="B5:B6"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="F3:H3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>